<commit_message>
Earnings Season Q125 part 1
Mostly tech and automotive
</commit_message>
<xml_diff>
--- a/Financial Analysis/AXP.xlsx
+++ b/Financial Analysis/AXP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\antos\Desktop\Financial Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69CD0A29-597B-457F-8503-A119CD2BA176}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5A31F86-7A22-49EC-A532-A26ADC230F71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{7753066E-724B-42EB-9AF0-1E4829C95CCE}"/>
   </bookViews>
@@ -825,7 +825,7 @@
       </c>
       <c r="G3" s="11">
         <f ca="1">TODAY()</f>
-        <v>45769</v>
+        <v>45782</v>
       </c>
       <c r="H3" s="11">
         <v>45856</v>
@@ -1496,7 +1496,7 @@
         <v>16</v>
       </c>
       <c r="C8" s="3">
-        <f t="shared" ref="C8:R8" si="5">SUM(C3:C6)</f>
+        <f t="shared" ref="C8:N8" si="5">SUM(C3:C6)</f>
         <v>9536</v>
       </c>
       <c r="D8" s="3">
@@ -1787,7 +1787,7 @@
         <v>2100.14</v>
       </c>
       <c r="R10" s="3">
-        <f t="shared" ref="Q10:R10" si="9">N10*0.99</f>
+        <f t="shared" ref="R10" si="9">N10*0.99</f>
         <v>2018.61</v>
       </c>
       <c r="V10" s="3">
@@ -4156,47 +4156,47 @@
         <v>702.5</v>
       </c>
       <c r="Z28" s="3">
-        <f>700.6</f>
+        <f t="shared" ref="Z28:AJ28" si="41">700.6</f>
         <v>700.6</v>
       </c>
       <c r="AA28" s="3">
-        <f>700.6</f>
+        <f t="shared" si="41"/>
         <v>700.6</v>
       </c>
       <c r="AB28" s="3">
-        <f>700.6</f>
+        <f t="shared" si="41"/>
         <v>700.6</v>
       </c>
       <c r="AC28" s="3">
-        <f>700.6</f>
+        <f t="shared" si="41"/>
         <v>700.6</v>
       </c>
       <c r="AD28" s="3">
-        <f>700.6</f>
+        <f t="shared" si="41"/>
         <v>700.6</v>
       </c>
       <c r="AE28" s="3">
-        <f>700.6</f>
+        <f t="shared" si="41"/>
         <v>700.6</v>
       </c>
       <c r="AF28" s="3">
-        <f>700.6</f>
+        <f t="shared" si="41"/>
         <v>700.6</v>
       </c>
       <c r="AG28" s="3">
-        <f>700.6</f>
+        <f t="shared" si="41"/>
         <v>700.6</v>
       </c>
       <c r="AH28" s="3">
-        <f>700.6</f>
+        <f t="shared" si="41"/>
         <v>700.6</v>
       </c>
       <c r="AI28" s="3">
-        <f>700.6</f>
+        <f t="shared" si="41"/>
         <v>700.6</v>
       </c>
       <c r="AJ28" s="3">
-        <f>700.6</f>
+        <f t="shared" si="41"/>
         <v>700.6</v>
       </c>
     </row>
@@ -4205,67 +4205,67 @@
         <v>35</v>
       </c>
       <c r="C29" s="6">
-        <f t="shared" ref="C29:L29" si="41">C27/C28</f>
+        <f t="shared" ref="C29:L29" si="42">C27/C28</f>
         <v>2.9525953017302013</v>
       </c>
       <c r="D29" s="6">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>2.762695175130117</v>
       </c>
       <c r="E29" s="6">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>2.643128428752286</v>
       </c>
       <c r="F29" s="6">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>2.2112814741876496</v>
       </c>
       <c r="G29" s="6">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>2.5545083696722464</v>
       </c>
       <c r="H29" s="6">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>3.0580953720635815</v>
       </c>
       <c r="I29" s="6">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>3.4477422984948656</v>
       </c>
       <c r="J29" s="6">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>2.7190884793923198</v>
       </c>
       <c r="K29" s="6">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>3.4280489520326349</v>
       </c>
       <c r="L29" s="6">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>4.2411028274018854</v>
       </c>
       <c r="M29" s="6">
-        <f t="shared" ref="M29:N29" si="42">M27/M28</f>
+        <f t="shared" ref="M29:N29" si="43">M27/M28</f>
         <v>3.5590573537762635</v>
       </c>
       <c r="N29" s="6">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>3.0889679715302489</v>
       </c>
       <c r="O29" s="6">
-        <f t="shared" ref="O29:R29" si="43">O27/O28</f>
+        <f t="shared" ref="O29:R29" si="44">O27/O28</f>
         <v>3.6882671995432483</v>
       </c>
       <c r="P29" s="6">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>4.2491010362546389</v>
       </c>
       <c r="Q29" s="6">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>4.1398780673708258</v>
       </c>
       <c r="R29" s="6">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>3.2876195047102454</v>
       </c>
       <c r="V29" s="6">
@@ -4289,43 +4289,43 @@
         <v>15.36486580787896</v>
       </c>
       <c r="AA29" s="6">
-        <f t="shared" ref="AA29:AJ29" si="44">AA27/AA28</f>
+        <f t="shared" ref="AA29:AJ29" si="45">AA27/AA28</f>
         <v>17.39878917156723</v>
       </c>
       <c r="AB29" s="6">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>17.956976623317157</v>
       </c>
       <c r="AC29" s="6">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>18.376309388341078</v>
       </c>
       <c r="AD29" s="6">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>18.678748708795972</v>
       </c>
       <c r="AE29" s="6">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>18.947818379640161</v>
       </c>
       <c r="AF29" s="6">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>19.179671888071024</v>
       </c>
       <c r="AG29" s="6">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>19.414691438078872</v>
       </c>
       <c r="AH29" s="6">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>19.652925640209354</v>
       </c>
       <c r="AI29" s="6">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>19.894423930116133</v>
       </c>
       <c r="AJ29" s="6">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>20.139236583592066</v>
       </c>
     </row>
@@ -4334,51 +4334,51 @@
         <v>67</v>
       </c>
       <c r="G31" s="7">
-        <f t="shared" ref="G31:K31" si="45">G3/C3-1</f>
+        <f t="shared" ref="G31:K31" si="46">G3/C3-1</f>
         <v>0.16269202633504021</v>
       </c>
       <c r="H31" s="7">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>7.7225962149117144E-2</v>
       </c>
       <c r="I31" s="7">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>7.1355759429153842E-2</v>
       </c>
       <c r="J31" s="7">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>4.8515214469021073E-2</v>
       </c>
       <c r="K31" s="7">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>5.4485969548257129E-2</v>
       </c>
       <c r="L31" s="7">
-        <f>L3/H3-1</f>
+        <f t="shared" ref="L31:R31" si="47">L3/H3-1</f>
         <v>4.4098573281452724E-2</v>
       </c>
       <c r="M31" s="7">
-        <f>M3/I3-1</f>
+        <f t="shared" si="47"/>
         <v>4.4243577545195034E-2</v>
       </c>
       <c r="N31" s="7">
-        <f>N3/J3-1</f>
+        <f t="shared" si="47"/>
         <v>6.9580419580419495E-2</v>
       </c>
       <c r="O31" s="7">
-        <f>O3/K3-1</f>
+        <f t="shared" si="47"/>
         <v>4.3317422434367536E-2</v>
       </c>
       <c r="P31" s="7">
-        <f>P3/L3-1</f>
+        <f t="shared" si="47"/>
         <v>6.0000000000000053E-2</v>
       </c>
       <c r="Q31" s="7">
-        <f>Q3/M3-1</f>
+        <f t="shared" si="47"/>
         <v>6.0000000000000053E-2</v>
       </c>
       <c r="R31" s="7">
-        <f>R3/N3-1</f>
+        <f t="shared" si="47"/>
         <v>4.0000000000000036E-2</v>
       </c>
       <c r="W31" s="7">
@@ -4386,55 +4386,55 @@
         <v>0.76518892844837483</v>
       </c>
       <c r="X31" s="7">
-        <f t="shared" ref="X31:AJ31" si="46">X3/W3-1</f>
+        <f t="shared" ref="X31:AJ31" si="48">X3/W3-1</f>
         <v>8.7088064022902589E-2</v>
       </c>
       <c r="Y31" s="7">
-        <f t="shared" si="46"/>
+        <f t="shared" si="48"/>
         <v>5.3148192482643131E-2</v>
       </c>
       <c r="Z31" s="7">
-        <f t="shared" si="46"/>
+        <f t="shared" si="48"/>
         <v>5.0812116390088979E-2</v>
       </c>
       <c r="AA31" s="7">
-        <f t="shared" si="46"/>
+        <f t="shared" si="48"/>
         <v>2.0000000000000018E-2</v>
       </c>
       <c r="AB31" s="7">
-        <f t="shared" si="46"/>
+        <f t="shared" si="48"/>
         <v>1.0000000000000009E-2</v>
       </c>
       <c r="AC31" s="7">
-        <f t="shared" si="46"/>
+        <f t="shared" si="48"/>
         <v>1.0000000000000009E-2</v>
       </c>
       <c r="AD31" s="7">
-        <f t="shared" si="46"/>
+        <f t="shared" si="48"/>
         <v>1.0000000000000009E-2</v>
       </c>
       <c r="AE31" s="7">
-        <f t="shared" si="46"/>
+        <f t="shared" si="48"/>
         <v>1.0000000000000009E-2</v>
       </c>
       <c r="AF31" s="7">
-        <f t="shared" si="46"/>
+        <f t="shared" si="48"/>
         <v>1.0000000000000009E-2</v>
       </c>
       <c r="AG31" s="7">
-        <f t="shared" si="46"/>
+        <f t="shared" si="48"/>
         <v>1.0000000000000009E-2</v>
       </c>
       <c r="AH31" s="7">
-        <f t="shared" si="46"/>
+        <f t="shared" si="48"/>
         <v>1.0000000000000009E-2</v>
       </c>
       <c r="AI31" s="7">
-        <f t="shared" si="46"/>
+        <f t="shared" si="48"/>
         <v>1.0000000000000009E-2</v>
       </c>
       <c r="AJ31" s="7">
-        <f t="shared" si="46"/>
+        <f t="shared" si="48"/>
         <v>1.0000000000000009E-2</v>
       </c>
     </row>
@@ -4443,31 +4443,31 @@
         <v>68</v>
       </c>
       <c r="G32" s="7">
-        <f t="shared" ref="G32:M32" si="47">G4/C4-1</f>
+        <f t="shared" ref="G32:M32" si="49">G4/C4-1</f>
         <v>0.2037947997189038</v>
       </c>
       <c r="H32" s="7">
-        <f t="shared" si="47"/>
+        <f t="shared" si="49"/>
         <v>0.20796758946657667</v>
       </c>
       <c r="I32" s="7">
-        <f t="shared" si="47"/>
+        <f t="shared" si="49"/>
         <v>0.19792342634652815</v>
       </c>
       <c r="J32" s="7">
-        <f t="shared" si="47"/>
+        <f t="shared" si="49"/>
         <v>0.17353846153846164</v>
       </c>
       <c r="K32" s="7">
-        <f t="shared" si="47"/>
+        <f t="shared" si="49"/>
         <v>0.15236427320490376</v>
       </c>
       <c r="L32" s="7">
-        <f t="shared" si="47"/>
+        <f t="shared" si="49"/>
         <v>0.1514812744550027</v>
       </c>
       <c r="M32" s="7">
-        <f t="shared" si="47"/>
+        <f t="shared" si="49"/>
         <v>0.17551462621885161</v>
       </c>
       <c r="N32" s="7">
@@ -4495,55 +4495,55 @@
         <v>0.57621397039729949</v>
       </c>
       <c r="X32" s="7">
-        <f>X4/W4-1</f>
+        <f t="shared" ref="X32:AJ32" si="50">X4/W4-1</f>
         <v>0.19522240527182877</v>
       </c>
       <c r="Y32" s="7">
-        <f>Y4/X4-1</f>
+        <f t="shared" si="50"/>
         <v>0.16457615437629225</v>
       </c>
       <c r="Z32" s="7">
-        <f>Z4/Y4-1</f>
+        <f t="shared" si="50"/>
         <v>0.15456858799857986</v>
       </c>
       <c r="AA32" s="7">
-        <f>AA4/Z4-1</f>
+        <f t="shared" si="50"/>
         <v>9.000000000000008E-2</v>
       </c>
       <c r="AB32" s="7">
-        <f>AB4/AA4-1</f>
+        <f t="shared" si="50"/>
         <v>7.0000000000000062E-2</v>
       </c>
       <c r="AC32" s="7">
-        <f>AC4/AB4-1</f>
+        <f t="shared" si="50"/>
         <v>5.0000000000000044E-2</v>
       </c>
       <c r="AD32" s="7">
-        <f>AD4/AC4-1</f>
+        <f t="shared" si="50"/>
         <v>4.0000000000000036E-2</v>
       </c>
       <c r="AE32" s="7">
-        <f>AE4/AD4-1</f>
+        <f t="shared" si="50"/>
         <v>3.0000000000000027E-2</v>
       </c>
       <c r="AF32" s="7">
-        <f>AF4/AE4-1</f>
+        <f t="shared" si="50"/>
         <v>2.0000000000000018E-2</v>
       </c>
       <c r="AG32" s="7">
-        <f>AG4/AF4-1</f>
+        <f t="shared" si="50"/>
         <v>2.0000000000000018E-2</v>
       </c>
       <c r="AH32" s="7">
-        <f>AH4/AG4-1</f>
+        <f t="shared" si="50"/>
         <v>2.0000000000000018E-2</v>
       </c>
       <c r="AI32" s="7">
-        <f>AI4/AH4-1</f>
+        <f t="shared" si="50"/>
         <v>2.0000000000000018E-2</v>
       </c>
       <c r="AJ32" s="7">
-        <f>AJ4/AI4-1</f>
+        <f t="shared" si="50"/>
         <v>2.0000000000000018E-2</v>
       </c>
     </row>
@@ -4552,31 +4552,31 @@
         <v>69</v>
       </c>
       <c r="G33" s="7">
-        <f t="shared" ref="G33:M33" si="48">G5/C5-1</f>
+        <f t="shared" ref="G33:M33" si="51">G5/C5-1</f>
         <v>0.3443708609271523</v>
       </c>
       <c r="H33" s="7">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v>-2.6086956521739091E-2</v>
       </c>
       <c r="I33" s="7">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v>7.8699743370401976E-2</v>
       </c>
       <c r="J33" s="7">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v>9.5681625740897447E-2</v>
       </c>
       <c r="K33" s="7">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v>6.075533661740562E-2</v>
       </c>
       <c r="L33" s="7">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v>3.8961038961038863E-2</v>
       </c>
       <c r="M33" s="7">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v>4.7581284694686587E-3</v>
       </c>
       <c r="N33" s="7">
@@ -4588,15 +4588,15 @@
         <v>2.6221692491060766E-2</v>
       </c>
       <c r="P33" s="7">
-        <f>P5/L5-1</f>
+        <f t="shared" ref="P33:R34" si="52">P5/L5-1</f>
         <v>2.0000000000000018E-2</v>
       </c>
       <c r="Q33" s="7">
-        <f>Q5/M5-1</f>
+        <f t="shared" si="52"/>
         <v>2.0000000000000018E-2</v>
       </c>
       <c r="R33" s="7">
-        <f>R5/N5-1</f>
+        <f t="shared" si="52"/>
         <v>2.0000000000000018E-2</v>
       </c>
       <c r="W33" s="7">
@@ -4616,43 +4616,43 @@
         <v>2.3970436067997092E-2</v>
       </c>
       <c r="AA33" s="7">
-        <f t="shared" ref="AA33:AJ33" si="49">AA7/Z7-1</f>
+        <f t="shared" ref="AA33:AJ33" si="53">AA7/Z7-1</f>
         <v>2.0000000000000018E-2</v>
       </c>
       <c r="AB33" s="7">
-        <f t="shared" si="49"/>
+        <f t="shared" si="53"/>
         <v>1.0000000000000009E-2</v>
       </c>
       <c r="AC33" s="7">
-        <f t="shared" si="49"/>
+        <f t="shared" si="53"/>
         <v>1.0000000000000009E-2</v>
       </c>
       <c r="AD33" s="7">
-        <f t="shared" si="49"/>
+        <f t="shared" si="53"/>
         <v>1.0000000000000009E-2</v>
       </c>
       <c r="AE33" s="7">
-        <f t="shared" si="49"/>
+        <f t="shared" si="53"/>
         <v>1.0000000000000009E-2</v>
       </c>
       <c r="AF33" s="7">
-        <f t="shared" si="49"/>
+        <f t="shared" si="53"/>
         <v>1.0000000000000009E-2</v>
       </c>
       <c r="AG33" s="7">
-        <f t="shared" si="49"/>
+        <f t="shared" si="53"/>
         <v>1.0000000000000009E-2</v>
       </c>
       <c r="AH33" s="7">
-        <f t="shared" si="49"/>
+        <f t="shared" si="53"/>
         <v>1.0000000000000009E-2</v>
       </c>
       <c r="AI33" s="7">
-        <f t="shared" si="49"/>
+        <f t="shared" si="53"/>
         <v>1.0000000000000009E-2</v>
       </c>
       <c r="AJ33" s="7">
-        <f t="shared" si="49"/>
+        <f t="shared" si="53"/>
         <v>1.0000000000000009E-2</v>
       </c>
     </row>
@@ -4661,31 +4661,31 @@
         <v>70</v>
       </c>
       <c r="G34" s="7">
-        <f t="shared" ref="G34:M34" si="50">G6/C6-1</f>
+        <f t="shared" ref="G34:M34" si="54">G6/C6-1</f>
         <v>0.12903225806451624</v>
       </c>
       <c r="H34" s="7">
-        <f t="shared" si="50"/>
+        <f t="shared" si="54"/>
         <v>7.4519230769230838E-2</v>
       </c>
       <c r="I34" s="7">
-        <f t="shared" si="50"/>
+        <f t="shared" si="54"/>
         <v>9.52380952380949E-3</v>
       </c>
       <c r="J34" s="7">
-        <f t="shared" si="50"/>
+        <f t="shared" si="54"/>
         <v>-3.4965034965035002E-2</v>
       </c>
       <c r="K34" s="7">
-        <f t="shared" si="50"/>
+        <f t="shared" si="54"/>
         <v>-8.0952380952380998E-2</v>
       </c>
       <c r="L34" s="7">
-        <f t="shared" si="50"/>
+        <f t="shared" si="54"/>
         <v>-8.7248322147650992E-2</v>
       </c>
       <c r="M34" s="7">
-        <f t="shared" si="50"/>
+        <f t="shared" si="54"/>
         <v>-2.5943396226415061E-2</v>
       </c>
       <c r="N34" s="7">
@@ -4694,15 +4694,15 @@
       </c>
       <c r="O34" s="7"/>
       <c r="P34" s="7">
-        <f>P6/L6-1</f>
+        <f t="shared" si="52"/>
         <v>4.0000000000000036E-2</v>
       </c>
       <c r="Q34" s="7">
-        <f>Q6/M6-1</f>
+        <f t="shared" si="52"/>
         <v>4.0000000000000036E-2</v>
       </c>
       <c r="R34" s="7">
-        <f>R6/N6-1</f>
+        <f t="shared" si="52"/>
         <v>2.0000000000000018E-2</v>
       </c>
       <c r="W34" s="7">
@@ -4734,107 +4734,107 @@
         <v>65</v>
       </c>
       <c r="G35" s="7">
-        <f t="shared" ref="G35:K37" si="51">G9/C9-1</f>
+        <f t="shared" ref="G35:K37" si="55">G9/C9-1</f>
         <v>0.75238095238095237</v>
       </c>
       <c r="H35" s="7">
-        <f t="shared" ref="H35:H36" si="52">H9/D9-1</f>
+        <f t="shared" ref="H35:H36" si="56">H9/D9-1</f>
         <v>0.70596641657734915</v>
       </c>
       <c r="I35" s="7">
-        <f t="shared" ref="I35:I36" si="53">I9/E9-1</f>
+        <f t="shared" ref="I35:I36" si="57">I9/E9-1</f>
         <v>0.55305275637225848</v>
       </c>
       <c r="J35" s="7">
-        <f t="shared" ref="J35:J36" si="54">J9/F9-1</f>
+        <f t="shared" ref="J35:J36" si="58">J9/F9-1</f>
         <v>0.40025220680958395</v>
       </c>
       <c r="K35" s="7">
-        <f t="shared" ref="K35:K36" si="55">K9/G9-1</f>
+        <f t="shared" ref="K35:K36" si="59">K9/G9-1</f>
         <v>0.30774456521739135</v>
       </c>
       <c r="L35" s="7">
-        <f t="shared" ref="L35:L36" si="56">L9/H9-1</f>
+        <f t="shared" ref="L35:L36" si="60">L9/H9-1</f>
         <v>0.21340314136125649</v>
       </c>
       <c r="M35" s="7">
-        <f t="shared" ref="M35:M36" si="57">M9/I9-1</f>
+        <f t="shared" ref="M35:M36" si="61">M9/I9-1</f>
         <v>0.17347328244274807</v>
       </c>
       <c r="N35" s="7">
-        <f t="shared" ref="N35:N36" si="58">N9/J9-1</f>
+        <f t="shared" ref="N35:N36" si="62">N9/J9-1</f>
         <v>9.4560518731988452E-2</v>
       </c>
       <c r="O35" s="7">
-        <f t="shared" ref="O35:O37" si="59">O9/K9-1</f>
+        <f t="shared" ref="O35:O37" si="63">O9/K9-1</f>
         <v>6.2337662337662358E-2</v>
       </c>
       <c r="P35" s="7">
-        <f t="shared" ref="P35:P37" si="60">P9/L9-1</f>
+        <f t="shared" ref="P35:P37" si="64">P9/L9-1</f>
         <v>6.0000000000000053E-2</v>
       </c>
       <c r="Q35" s="7">
-        <f t="shared" ref="Q35:Q37" si="61">Q9/M9-1</f>
+        <f t="shared" ref="Q35:Q37" si="65">Q9/M9-1</f>
         <v>2.0000000000000018E-2</v>
       </c>
       <c r="R35" s="7">
-        <f t="shared" ref="R35:R37" si="62">R9/N9-1</f>
+        <f t="shared" ref="R35:R37" si="66">R9/N9-1</f>
         <v>4.0000000000000036E-2</v>
       </c>
       <c r="W35" s="7">
-        <f t="shared" ref="W35:AJ35" si="63">W9/V9-1</f>
+        <f t="shared" ref="W35:AJ35" si="67">W9/V9-1</f>
         <v>0.90833710236695309</v>
       </c>
       <c r="X35" s="7">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>0.57868541633749415</v>
       </c>
       <c r="Y35" s="7">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>0.19076214782565182</v>
       </c>
       <c r="Z35" s="7">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>4.5122924984240198E-2</v>
       </c>
       <c r="AA35" s="7">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>5.0000000000000044E-2</v>
       </c>
       <c r="AB35" s="7">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>3.0000000000000027E-2</v>
       </c>
       <c r="AC35" s="7">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>2.0000000000000018E-2</v>
       </c>
       <c r="AD35" s="7">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>1.0000000000000009E-2</v>
       </c>
       <c r="AE35" s="7">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>1.0000000000000009E-2</v>
       </c>
       <c r="AF35" s="7">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>1.0000000000000009E-2</v>
       </c>
       <c r="AG35" s="7">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>1.0000000000000009E-2</v>
       </c>
       <c r="AH35" s="7">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>1.0000000000000009E-2</v>
       </c>
       <c r="AI35" s="7">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>1.0000000000000009E-2</v>
       </c>
       <c r="AJ35" s="7">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>1.0000000000000009E-2</v>
       </c>
     </row>
@@ -4843,107 +4843,107 @@
         <v>71</v>
       </c>
       <c r="G36" s="7">
-        <f t="shared" si="51"/>
+        <f t="shared" si="55"/>
         <v>3.4641744548286608</v>
       </c>
       <c r="H36" s="7">
-        <f t="shared" si="52"/>
+        <f t="shared" si="56"/>
         <v>2.8041002277904328</v>
       </c>
       <c r="I36" s="7">
-        <f t="shared" si="53"/>
+        <f t="shared" si="57"/>
         <v>1.2587939698492461</v>
       </c>
       <c r="J36" s="7">
-        <f t="shared" si="54"/>
+        <f t="shared" si="58"/>
         <v>0.61391880695940348</v>
       </c>
       <c r="K36" s="7">
-        <f t="shared" si="55"/>
+        <f t="shared" si="59"/>
         <v>0.39986043265875781</v>
       </c>
       <c r="L36" s="7">
-        <f t="shared" si="56"/>
+        <f t="shared" si="60"/>
         <v>0.23592814371257487</v>
       </c>
       <c r="M36" s="7">
-        <f t="shared" si="57"/>
+        <f t="shared" si="61"/>
         <v>0.19187986651835365</v>
       </c>
       <c r="N36" s="7">
-        <f t="shared" si="58"/>
+        <f t="shared" si="62"/>
         <v>4.6714579055441519E-2</v>
       </c>
       <c r="O36" s="7">
-        <f t="shared" si="59"/>
+        <f t="shared" si="63"/>
         <v>-1.9940179461615193E-2</v>
       </c>
       <c r="P36" s="7">
-        <f t="shared" si="60"/>
+        <f t="shared" si="64"/>
         <v>-1.0000000000000009E-2</v>
       </c>
       <c r="Q36" s="7">
-        <f t="shared" si="61"/>
+        <f t="shared" si="65"/>
         <v>-2.0000000000000018E-2</v>
       </c>
       <c r="R36" s="7">
-        <f t="shared" si="62"/>
+        <f t="shared" si="66"/>
         <v>-1.0000000000000009E-2</v>
       </c>
       <c r="W36" s="7">
-        <f t="shared" ref="W36:AJ36" si="64">W10/V10-1</f>
+        <f t="shared" ref="W36:AJ36" si="68">W10/V10-1</f>
         <v>1.7880928355196772</v>
       </c>
       <c r="X36" s="7">
-        <f t="shared" si="64"/>
+        <f t="shared" si="68"/>
         <v>1.4788273615635181</v>
       </c>
       <c r="Y36" s="7">
-        <f t="shared" si="64"/>
+        <f t="shared" si="68"/>
         <v>0.20484742298145719</v>
       </c>
       <c r="Z36" s="7">
-        <f t="shared" si="64"/>
+        <f t="shared" si="68"/>
         <v>-1.5013330101793509E-2</v>
       </c>
       <c r="AA36" s="7">
-        <f t="shared" si="64"/>
+        <f t="shared" si="68"/>
         <v>5.0000000000000044E-2</v>
       </c>
       <c r="AB36" s="7">
-        <f t="shared" si="64"/>
+        <f t="shared" si="68"/>
         <v>3.0000000000000027E-2</v>
       </c>
       <c r="AC36" s="7">
-        <f t="shared" si="64"/>
+        <f t="shared" si="68"/>
         <v>2.0000000000000018E-2</v>
       </c>
       <c r="AD36" s="7">
-        <f t="shared" si="64"/>
+        <f t="shared" si="68"/>
         <v>1.0000000000000009E-2</v>
       </c>
       <c r="AE36" s="7">
-        <f t="shared" si="64"/>
+        <f t="shared" si="68"/>
         <v>1.0000000000000009E-2</v>
       </c>
       <c r="AF36" s="7">
-        <f t="shared" si="64"/>
+        <f t="shared" si="68"/>
         <v>1.0000000000000009E-2</v>
       </c>
       <c r="AG36" s="7">
-        <f t="shared" si="64"/>
+        <f t="shared" si="68"/>
         <v>1.0000000000000009E-2</v>
       </c>
       <c r="AH36" s="7">
-        <f t="shared" si="64"/>
+        <f t="shared" si="68"/>
         <v>1.0000000000000009E-2</v>
       </c>
       <c r="AI36" s="7">
-        <f t="shared" si="64"/>
+        <f t="shared" si="68"/>
         <v>1.0000000000000009E-2</v>
       </c>
       <c r="AJ36" s="7">
-        <f t="shared" si="64"/>
+        <f t="shared" si="68"/>
         <v>1.0000000000000009E-2</v>
       </c>
     </row>
@@ -4952,23 +4952,23 @@
         <v>66</v>
       </c>
       <c r="G37" s="7">
-        <f t="shared" si="51"/>
+        <f t="shared" si="55"/>
         <v>0.35652569349704422</v>
       </c>
       <c r="H37" s="7">
-        <f t="shared" si="51"/>
+        <f t="shared" si="55"/>
         <v>0.31567796610169485</v>
       </c>
       <c r="I37" s="7">
-        <f t="shared" si="51"/>
+        <f t="shared" si="55"/>
         <v>0.33514352211016285</v>
       </c>
       <c r="J37" s="7">
-        <f t="shared" si="51"/>
+        <f t="shared" si="55"/>
         <v>0.30674401740391599</v>
       </c>
       <c r="K37" s="7">
-        <f t="shared" si="51"/>
+        <f t="shared" si="55"/>
         <v>0.26349312772376798</v>
       </c>
       <c r="L37" s="7">
@@ -4980,31 +4980,31 @@
         <v>0.16385822196397437</v>
       </c>
       <c r="N37" s="7">
-        <f t="shared" ref="N37" si="65">N11/J11-1</f>
+        <f t="shared" ref="N37" si="69">N11/J11-1</f>
         <v>0.12042175360710328</v>
       </c>
       <c r="O37" s="7">
-        <f t="shared" si="59"/>
+        <f t="shared" si="63"/>
         <v>0.10612894667020423</v>
       </c>
       <c r="P37" s="7">
-        <f t="shared" si="60"/>
+        <f t="shared" si="64"/>
         <v>9.8734584450402396E-2</v>
       </c>
       <c r="Q37" s="7">
-        <f t="shared" si="61"/>
+        <f t="shared" si="65"/>
         <v>4.1397903145282022E-2</v>
       </c>
       <c r="R37" s="7">
-        <f t="shared" si="62"/>
+        <f t="shared" si="66"/>
         <v>6.5247647350173521E-2</v>
       </c>
       <c r="W37" s="7">
-        <f t="shared" ref="W37:X37" si="66">W11/V11-1</f>
+        <f t="shared" ref="W37:X37" si="70">W11/V11-1</f>
         <v>0.75381070542360873</v>
       </c>
       <c r="X37" s="7">
-        <f t="shared" si="66"/>
+        <f t="shared" si="70"/>
         <v>0.32733703890853971</v>
       </c>
       <c r="Y37" s="7">
@@ -5012,47 +5012,47 @@
         <v>0.18341708542713575</v>
       </c>
       <c r="Z37" s="7">
-        <f t="shared" ref="Z37:AJ37" si="67">Z11/Y11-1</f>
+        <f t="shared" ref="Z37:AJ37" si="71">Z11/Y11-1</f>
         <v>7.7050119024641095E-2</v>
       </c>
       <c r="AA37" s="7">
-        <f t="shared" si="67"/>
+        <f t="shared" si="71"/>
         <v>5.0000000000000266E-2</v>
       </c>
       <c r="AB37" s="7">
-        <f t="shared" si="67"/>
+        <f t="shared" si="71"/>
         <v>2.9999999999999805E-2</v>
       </c>
       <c r="AC37" s="7">
-        <f t="shared" si="67"/>
+        <f t="shared" si="71"/>
         <v>2.0000000000000018E-2</v>
       </c>
       <c r="AD37" s="7">
-        <f t="shared" si="67"/>
+        <f t="shared" si="71"/>
         <v>1.0000000000000009E-2</v>
       </c>
       <c r="AE37" s="7">
-        <f t="shared" si="67"/>
+        <f t="shared" si="71"/>
         <v>1.0000000000000009E-2</v>
       </c>
       <c r="AF37" s="7">
-        <f t="shared" si="67"/>
+        <f t="shared" si="71"/>
         <v>1.0000000000000009E-2</v>
       </c>
       <c r="AG37" s="7">
-        <f t="shared" si="67"/>
+        <f t="shared" si="71"/>
         <v>1.0000000000000009E-2</v>
       </c>
       <c r="AH37" s="7">
-        <f t="shared" si="67"/>
+        <f t="shared" si="71"/>
         <v>1.0000000000000009E-2</v>
       </c>
       <c r="AI37" s="7">
-        <f t="shared" si="67"/>
+        <f t="shared" si="71"/>
         <v>1.0000000000000009E-2</v>
       </c>
       <c r="AJ37" s="7">
-        <f t="shared" si="67"/>
+        <f t="shared" si="71"/>
         <v>9.9999999999997868E-3</v>
       </c>
     </row>
@@ -5065,23 +5065,23 @@
       <c r="E38" s="7"/>
       <c r="F38" s="7"/>
       <c r="G38" s="7">
-        <f t="shared" ref="G38:K38" si="68">G16/C16-1</f>
+        <f t="shared" ref="G38:K38" si="72">G16/C16-1</f>
         <v>0.30341738553417374</v>
       </c>
       <c r="H38" s="7">
-        <f t="shared" si="68"/>
+        <f t="shared" si="72"/>
         <v>0.20890559491108873</v>
       </c>
       <c r="I38" s="7">
-        <f t="shared" si="68"/>
+        <f t="shared" si="72"/>
         <v>0.19697603121516161</v>
       </c>
       <c r="J38" s="7">
-        <f t="shared" si="68"/>
+        <f t="shared" si="72"/>
         <v>0.15367613599427932</v>
       </c>
       <c r="K38" s="7">
-        <f t="shared" si="68"/>
+        <f t="shared" si="72"/>
         <v>0.13319333078783258</v>
       </c>
       <c r="L38" s="7">
@@ -5089,27 +5089,27 @@
         <v>0.10003587658454904</v>
       </c>
       <c r="M38" s="7">
-        <f t="shared" ref="M38:N38" si="69">M16/I16-1</f>
+        <f t="shared" ref="M38:N38" si="73">M16/I16-1</f>
         <v>9.3136969555853044E-2</v>
       </c>
       <c r="N38" s="7">
-        <f t="shared" si="69"/>
+        <f t="shared" si="73"/>
         <v>8.2887248549050607E-2</v>
       </c>
       <c r="O38" s="7">
-        <f t="shared" ref="O38" si="70">O16/K16-1</f>
+        <f t="shared" ref="O38" si="74">O16/K16-1</f>
         <v>6.3233559836019637E-2</v>
       </c>
       <c r="P38" s="7">
-        <f t="shared" ref="P38" si="71">P16/L16-1</f>
+        <f t="shared" ref="P38" si="75">P16/L16-1</f>
         <v>6.7970864814915544E-2</v>
       </c>
       <c r="Q38" s="7">
-        <f t="shared" ref="Q38" si="72">Q16/M16-1</f>
+        <f t="shared" ref="Q38" si="76">Q16/M16-1</f>
         <v>5.416369348740635E-2</v>
       </c>
       <c r="R38" s="7">
-        <f t="shared" ref="R38" si="73">R16/N16-1</f>
+        <f t="shared" ref="R38" si="77">R16/N16-1</f>
         <v>4.8724633156415731E-2</v>
       </c>
       <c r="V38" s="7"/>
@@ -5118,55 +5118,55 @@
         <v>0.78136809069365265</v>
       </c>
       <c r="X38" s="7">
-        <f t="shared" ref="X38:AJ38" si="74">X16/W16-1</f>
+        <f t="shared" ref="X38:AJ38" si="78">X16/W16-1</f>
         <v>0.21103820224719105</v>
       </c>
       <c r="Y38" s="7">
-        <f t="shared" si="74"/>
+        <f t="shared" si="78"/>
         <v>0.10149337925301349</v>
       </c>
       <c r="Z38" s="7">
-        <f t="shared" si="74"/>
+        <f t="shared" si="78"/>
         <v>5.8354873923532002E-2</v>
       </c>
       <c r="AA38" s="7">
-        <f t="shared" si="74"/>
+        <f t="shared" si="78"/>
         <v>3.8195460161650763E-2</v>
       </c>
       <c r="AB38" s="7">
-        <f t="shared" si="74"/>
+        <f t="shared" si="78"/>
         <v>2.4230455888448077E-2</v>
       </c>
       <c r="AC38" s="7">
-        <f t="shared" si="74"/>
+        <f t="shared" si="78"/>
         <v>1.8670545596600974E-2</v>
       </c>
       <c r="AD38" s="7">
-        <f t="shared" si="74"/>
+        <f t="shared" si="78"/>
         <v>1.4213027022785152E-2</v>
       </c>
       <c r="AE38" s="7">
-        <f t="shared" si="74"/>
+        <f t="shared" si="78"/>
         <v>1.2880097170222538E-2</v>
       </c>
       <c r="AF38" s="7">
-        <f t="shared" si="74"/>
+        <f t="shared" si="78"/>
         <v>1.1464388575517015E-2</v>
       </c>
       <c r="AG38" s="7">
-        <f t="shared" si="74"/>
+        <f t="shared" si="78"/>
         <v>1.1476746353008771E-2</v>
       </c>
       <c r="AH38" s="7">
-        <f t="shared" si="74"/>
+        <f t="shared" si="78"/>
         <v>1.1489190221624312E-2</v>
       </c>
       <c r="AI38" s="7">
-        <f t="shared" si="74"/>
+        <f t="shared" si="78"/>
         <v>1.1501720473872545E-2</v>
       </c>
       <c r="AJ38" s="7">
-        <f t="shared" si="74"/>
+        <f t="shared" si="78"/>
         <v>1.1514337397896313E-2</v>
       </c>
     </row>
@@ -5175,39 +5175,39 @@
         <v>48</v>
       </c>
       <c r="C39" s="7">
-        <f t="shared" ref="C39:K39" si="75">C21/C16</f>
+        <f t="shared" ref="C39:K39" si="79">C21/C16</f>
         <v>0.57962840079628397</v>
       </c>
       <c r="D39" s="7">
-        <f t="shared" si="75"/>
+        <f t="shared" si="79"/>
         <v>0.52855284082694809</v>
       </c>
       <c r="E39" s="7">
-        <f t="shared" si="75"/>
+        <f t="shared" si="79"/>
         <v>0.50438963210702337</v>
       </c>
       <c r="F39" s="7">
-        <f t="shared" si="75"/>
+        <f t="shared" si="79"/>
         <v>0.47045439771175973</v>
       </c>
       <c r="G39" s="7">
-        <f t="shared" si="75"/>
+        <f t="shared" si="79"/>
         <v>0.45080819651266385</v>
       </c>
       <c r="H39" s="7">
-        <f t="shared" si="75"/>
+        <f t="shared" si="79"/>
         <v>0.45222434824204738</v>
       </c>
       <c r="I39" s="7">
-        <f t="shared" si="75"/>
+        <f t="shared" si="79"/>
         <v>0.46498632050759647</v>
       </c>
       <c r="J39" s="7">
-        <f t="shared" si="75"/>
+        <f t="shared" si="79"/>
         <v>0.44880824928156871</v>
       </c>
       <c r="K39" s="7">
-        <f t="shared" si="75"/>
+        <f t="shared" si="79"/>
         <v>0.46021227607120796</v>
       </c>
       <c r="L39" s="7">
@@ -5223,79 +5223,79 @@
         <v>0.44447913414507234</v>
       </c>
       <c r="O39" s="7">
-        <f t="shared" ref="O39:R39" si="76">O21/O16</f>
+        <f t="shared" ref="O39:R39" si="80">O21/O16</f>
         <v>0.45328262821528548</v>
       </c>
       <c r="P39" s="7">
-        <f t="shared" si="76"/>
+        <f t="shared" si="80"/>
         <v>0.44999999999999996</v>
       </c>
       <c r="Q39" s="7">
-        <f t="shared" si="76"/>
+        <f t="shared" si="80"/>
         <v>0.44999999999999996</v>
       </c>
       <c r="R39" s="7">
-        <f t="shared" si="76"/>
+        <f t="shared" si="80"/>
         <v>0.43999999999999989</v>
       </c>
       <c r="V39" s="7">
-        <f t="shared" ref="V39:AJ39" si="77">V21/V16</f>
+        <f t="shared" ref="V39:AJ39" si="81">V21/V16</f>
         <v>0.63312624095305192</v>
       </c>
       <c r="W39" s="7">
-        <f t="shared" si="77"/>
+        <f t="shared" si="81"/>
         <v>0.51732134831460674</v>
       </c>
       <c r="X39" s="7">
-        <f t="shared" si="77"/>
+        <f t="shared" si="81"/>
         <v>0.45424856006175407</v>
       </c>
       <c r="Y39" s="7">
-        <f t="shared" si="77"/>
+        <f t="shared" si="81"/>
         <v>0.45143596447487233</v>
       </c>
       <c r="Z39" s="7">
-        <f t="shared" si="77"/>
+        <f t="shared" si="81"/>
         <v>0.4482249822649631</v>
       </c>
       <c r="AA39" s="7">
-        <f t="shared" si="77"/>
+        <f t="shared" si="81"/>
         <v>0.45000000000000007</v>
       </c>
       <c r="AB39" s="7">
-        <f t="shared" si="77"/>
+        <f t="shared" si="81"/>
         <v>0.45</v>
       </c>
       <c r="AC39" s="7">
-        <f t="shared" si="77"/>
+        <f t="shared" si="81"/>
         <v>0.44999999999999996</v>
       </c>
       <c r="AD39" s="7">
-        <f t="shared" si="77"/>
+        <f t="shared" si="81"/>
         <v>0.44999999999999996</v>
       </c>
       <c r="AE39" s="7">
-        <f t="shared" si="77"/>
+        <f t="shared" si="81"/>
         <v>0.45</v>
       </c>
       <c r="AF39" s="7">
-        <f t="shared" si="77"/>
+        <f t="shared" si="81"/>
         <v>0.45000000000000007</v>
       </c>
       <c r="AG39" s="7">
-        <f t="shared" si="77"/>
+        <f t="shared" si="81"/>
         <v>0.44999999999999996</v>
       </c>
       <c r="AH39" s="7">
-        <f t="shared" si="77"/>
+        <f t="shared" si="81"/>
         <v>0.45</v>
       </c>
       <c r="AI39" s="7">
-        <f t="shared" si="77"/>
+        <f t="shared" si="81"/>
         <v>0.45000000000000007</v>
       </c>
       <c r="AJ39" s="7">
-        <f t="shared" si="77"/>
+        <f t="shared" si="81"/>
         <v>0.45</v>
       </c>
       <c r="AM39" s="1" t="s">
@@ -5310,39 +5310,39 @@
         <v>49</v>
       </c>
       <c r="C40" s="7">
-        <f t="shared" ref="C40:K40" si="78">C22/C16</f>
+        <f t="shared" ref="C40:K40" si="82">C22/C16</f>
         <v>0.10152621101526212</v>
       </c>
       <c r="D40" s="7">
-        <f t="shared" si="78"/>
+        <f t="shared" si="82"/>
         <v>0.10857308081538239</v>
       </c>
       <c r="E40" s="7">
-        <f t="shared" si="78"/>
+        <f t="shared" si="82"/>
         <v>0.10158862876254181</v>
       </c>
       <c r="F40" s="7">
-        <f t="shared" si="78"/>
+        <f t="shared" si="82"/>
         <v>8.2818695963076117E-2</v>
       </c>
       <c r="G40" s="7">
-        <f t="shared" si="78"/>
+        <f t="shared" si="82"/>
         <v>8.5337915234822453E-2</v>
       </c>
       <c r="H40" s="7">
-        <f t="shared" si="78"/>
+        <f t="shared" si="82"/>
         <v>8.4190385075340823E-2</v>
       </c>
       <c r="I40" s="7">
-        <f t="shared" si="78"/>
+        <f t="shared" si="82"/>
         <v>7.1948308981896497E-2</v>
       </c>
       <c r="J40" s="7">
-        <f t="shared" si="78"/>
+        <f t="shared" si="82"/>
         <v>6.9194793486223025E-2</v>
       </c>
       <c r="K40" s="7">
-        <f t="shared" si="78"/>
+        <f t="shared" si="82"/>
         <v>8.2888751614533615E-2</v>
       </c>
       <c r="L40" s="7">
@@ -5350,87 +5350,87 @@
         <v>8.0447899113985977E-2</v>
       </c>
       <c r="M40" s="7">
-        <f t="shared" ref="M40:N40" si="79">M22/M16</f>
+        <f t="shared" ref="M40:N40" si="83">M22/M16</f>
         <v>7.8278928590446772E-2</v>
       </c>
       <c r="N40" s="7">
-        <f t="shared" si="79"/>
+        <f t="shared" si="83"/>
         <v>8.3983765220106157E-2</v>
       </c>
       <c r="O40" s="7">
-        <f t="shared" ref="O40:R40" si="80">O22/O16</f>
+        <f t="shared" ref="O40:R40" si="84">O22/O16</f>
         <v>7.848729731157239E-2</v>
       </c>
       <c r="P40" s="7">
-        <f t="shared" si="80"/>
+        <f t="shared" si="84"/>
         <v>0.08</v>
       </c>
       <c r="Q40" s="7">
-        <f t="shared" si="80"/>
+        <f t="shared" si="84"/>
         <v>0.08</v>
       </c>
       <c r="R40" s="7">
-        <f t="shared" si="80"/>
+        <f t="shared" si="84"/>
         <v>0.08</v>
       </c>
       <c r="V40" s="7">
-        <f t="shared" ref="V40:AJ40" si="81">V22/V16</f>
+        <f t="shared" ref="V40:AJ40" si="85">V22/V16</f>
         <v>0.11868314865816948</v>
       </c>
       <c r="W40" s="7">
-        <f t="shared" si="81"/>
+        <f t="shared" si="85"/>
         <v>9.8121348314606741E-2</v>
       </c>
       <c r="X40" s="7">
-        <f t="shared" si="81"/>
+        <f t="shared" si="85"/>
         <v>7.7385547176533453E-2</v>
       </c>
       <c r="Y40" s="7">
-        <f t="shared" si="81"/>
+        <f t="shared" si="85"/>
         <v>8.1400520208622526E-2</v>
       </c>
       <c r="Z40" s="7">
-        <f t="shared" si="81"/>
+        <f t="shared" si="85"/>
         <v>7.9635303209599162E-2</v>
       </c>
       <c r="AA40" s="7">
-        <f t="shared" si="81"/>
+        <f t="shared" si="85"/>
         <v>0.08</v>
       </c>
       <c r="AB40" s="7">
-        <f t="shared" si="81"/>
+        <f t="shared" si="85"/>
         <v>0.08</v>
       </c>
       <c r="AC40" s="7">
-        <f t="shared" si="81"/>
+        <f t="shared" si="85"/>
         <v>0.08</v>
       </c>
       <c r="AD40" s="7">
-        <f t="shared" si="81"/>
+        <f t="shared" si="85"/>
         <v>0.08</v>
       </c>
       <c r="AE40" s="7">
-        <f t="shared" si="81"/>
+        <f t="shared" si="85"/>
         <v>0.08</v>
       </c>
       <c r="AF40" s="7">
-        <f t="shared" si="81"/>
+        <f t="shared" si="85"/>
         <v>0.08</v>
       </c>
       <c r="AG40" s="7">
-        <f t="shared" si="81"/>
+        <f t="shared" si="85"/>
         <v>0.08</v>
       </c>
       <c r="AH40" s="7">
-        <f t="shared" si="81"/>
+        <f t="shared" si="85"/>
         <v>0.08</v>
       </c>
       <c r="AI40" s="7">
-        <f t="shared" si="81"/>
+        <f t="shared" si="85"/>
         <v>0.08</v>
       </c>
       <c r="AJ40" s="7">
-        <f t="shared" si="81"/>
+        <f t="shared" si="85"/>
         <v>0.08</v>
       </c>
       <c r="AM40" s="1" t="s">
@@ -5449,23 +5449,23 @@
       <c r="E41" s="7"/>
       <c r="F41" s="7"/>
       <c r="G41" s="7">
-        <f t="shared" ref="G41:K41" si="82">G23/C23-1</f>
+        <f t="shared" ref="G41:K41" si="86">G23/C23-1</f>
         <v>0.2176541717049576</v>
       </c>
       <c r="H41" s="7">
-        <f t="shared" si="82"/>
+        <f t="shared" si="86"/>
         <v>3.2488986784140916E-2</v>
       </c>
       <c r="I41" s="7">
-        <f t="shared" si="82"/>
+        <f t="shared" si="86"/>
         <v>0.17105263157894735</v>
       </c>
       <c r="J41" s="7">
-        <f t="shared" si="82"/>
+        <f t="shared" si="86"/>
         <v>4.7689282202556527E-2</v>
       </c>
       <c r="K41" s="7">
-        <f t="shared" si="82"/>
+        <f t="shared" si="86"/>
         <v>4.170804369414105E-2</v>
       </c>
       <c r="L41" s="7">
@@ -5473,27 +5473,27 @@
         <v>3.9466666666666761E-2</v>
       </c>
       <c r="M41" s="7">
-        <f t="shared" ref="M41:N41" si="83">M23/I23-1</f>
+        <f t="shared" ref="M41:N41" si="87">M23/I23-1</f>
         <v>9.7703957010253362E-4</v>
       </c>
       <c r="N41" s="7">
-        <f t="shared" si="83"/>
+        <f t="shared" si="87"/>
         <v>-1.3608634443923018E-2</v>
       </c>
       <c r="O41" s="7">
-        <f t="shared" ref="O41" si="84">O23/K23-1</f>
+        <f t="shared" ref="O41" si="88">O23/K23-1</f>
         <v>1.048617731172552E-2</v>
       </c>
       <c r="P41" s="7">
-        <f t="shared" ref="P41" si="85">P23/L23-1</f>
+        <f t="shared" ref="P41" si="89">P23/L23-1</f>
         <v>-1.0000000000000009E-2</v>
       </c>
       <c r="Q41" s="7">
-        <f t="shared" ref="Q41" si="86">Q23/M23-1</f>
+        <f t="shared" ref="Q41" si="90">Q23/M23-1</f>
         <v>1.0000000000000009E-2</v>
       </c>
       <c r="R41" s="7">
-        <f t="shared" ref="R41" si="87">R23/N23-1</f>
+        <f t="shared" ref="R41" si="91">R23/N23-1</f>
         <v>1.0000000000000009E-2</v>
       </c>
       <c r="V41" s="7"/>
@@ -5502,55 +5502,55 @@
         <v>0.58133449629306577</v>
       </c>
       <c r="X41" s="7">
-        <f t="shared" ref="X41:AJ41" si="88">X23/W23-1</f>
+        <f t="shared" ref="X41:AJ41" si="92">X23/W23-1</f>
         <v>0.11238279095421944</v>
       </c>
       <c r="Y41" s="7">
-        <f t="shared" si="88"/>
+        <f t="shared" si="92"/>
         <v>1.6238998388496295E-2</v>
       </c>
       <c r="Z41" s="7">
-        <f t="shared" si="88"/>
+        <f t="shared" si="92"/>
         <v>5.3696023420346517E-3</v>
       </c>
       <c r="AA41" s="7">
-        <f t="shared" si="88"/>
+        <f t="shared" si="92"/>
         <v>2.0000000000000018E-2</v>
       </c>
       <c r="AB41" s="7">
-        <f t="shared" si="88"/>
+        <f t="shared" si="92"/>
         <v>1.0000000000000009E-2</v>
       </c>
       <c r="AC41" s="7">
-        <f t="shared" si="88"/>
+        <f t="shared" si="92"/>
         <v>1.0000000000000009E-2</v>
       </c>
       <c r="AD41" s="7">
-        <f t="shared" si="88"/>
+        <f t="shared" si="92"/>
         <v>1.0000000000000009E-2</v>
       </c>
       <c r="AE41" s="7">
-        <f t="shared" si="88"/>
+        <f t="shared" si="92"/>
         <v>1.0000000000000009E-2</v>
       </c>
       <c r="AF41" s="7">
-        <f t="shared" si="88"/>
+        <f t="shared" si="92"/>
         <v>1.0000000000000009E-2</v>
       </c>
       <c r="AG41" s="7">
-        <f t="shared" si="88"/>
+        <f t="shared" si="92"/>
         <v>1.0000000000000009E-2</v>
       </c>
       <c r="AH41" s="7">
-        <f t="shared" si="88"/>
+        <f t="shared" si="92"/>
         <v>1.0000000000000009E-2</v>
       </c>
       <c r="AI41" s="7">
-        <f t="shared" si="88"/>
+        <f t="shared" si="92"/>
         <v>1.0000000000000009E-2</v>
       </c>
       <c r="AJ41" s="7">
-        <f t="shared" si="88"/>
+        <f t="shared" si="92"/>
         <v>1.0000000000000009E-2</v>
       </c>
       <c r="AM41" s="1" t="s">
@@ -5566,39 +5566,39 @@
         <v>51</v>
       </c>
       <c r="C42" s="7">
-        <f t="shared" ref="C42:K42" si="89">C24/C16</f>
+        <f t="shared" ref="C42:K42" si="93">C24/C16</f>
         <v>0.11595885865958859</v>
       </c>
       <c r="D42" s="7">
-        <f t="shared" si="89"/>
+        <f t="shared" si="93"/>
         <v>0.104886511493422</v>
       </c>
       <c r="E42" s="7">
-        <f t="shared" si="89"/>
+        <f t="shared" si="93"/>
         <v>0.10967112597547381</v>
       </c>
       <c r="F42" s="7">
-        <f t="shared" si="89"/>
+        <f t="shared" si="93"/>
         <v>0.13378404732496912</v>
       </c>
       <c r="G42" s="7">
-        <f t="shared" si="89"/>
+        <f t="shared" si="93"/>
         <v>9.940180730558737E-2</v>
       </c>
       <c r="H42" s="7">
-        <f t="shared" si="89"/>
+        <f t="shared" si="93"/>
         <v>9.2441999521645543E-2</v>
       </c>
       <c r="I42" s="7">
-        <f t="shared" si="89"/>
+        <f t="shared" si="93"/>
         <v>9.3428022585715115E-2</v>
       </c>
       <c r="J42" s="7">
-        <f t="shared" si="89"/>
+        <f t="shared" si="93"/>
         <v>0.11799177325745197</v>
       </c>
       <c r="K42" s="7">
-        <f t="shared" si="89"/>
+        <f t="shared" si="93"/>
         <v>8.2888751614533615E-2</v>
       </c>
       <c r="L42" s="7">
@@ -5606,87 +5606,87 @@
         <v>5.6422242756971247E-2</v>
       </c>
       <c r="M42" s="7">
-        <f t="shared" ref="M42:N42" si="90">M24/M16</f>
+        <f t="shared" ref="M42:N42" si="94">M24/M16</f>
         <v>9.4786729857819899E-2</v>
       </c>
       <c r="N42" s="7">
-        <f t="shared" si="90"/>
+        <f t="shared" si="94"/>
         <v>0.10771152044957852</v>
       </c>
       <c r="O42" s="7">
-        <f t="shared" ref="O42:R42" si="91">O24/O16</f>
+        <f t="shared" ref="O42:R42" si="95">O24/O16</f>
         <v>8.693815031954788E-2</v>
       </c>
       <c r="P42" s="7">
-        <f t="shared" si="91"/>
+        <f t="shared" si="95"/>
         <v>0.08</v>
       </c>
       <c r="Q42" s="7">
-        <f t="shared" si="91"/>
+        <f t="shared" si="95"/>
         <v>0.08</v>
       </c>
       <c r="R42" s="7">
-        <f t="shared" si="91"/>
+        <f t="shared" si="95"/>
         <v>0.11</v>
       </c>
       <c r="V42" s="7">
-        <f t="shared" ref="V42:AJ42" si="92">V24/V16</f>
+        <f t="shared" ref="V42:AJ42" si="96">V24/V16</f>
         <v>9.9116121181067066E-2</v>
       </c>
       <c r="W42" s="7">
-        <f t="shared" si="92"/>
+        <f t="shared" si="96"/>
         <v>0.1165123595505618</v>
       </c>
       <c r="X42" s="7">
-        <f t="shared" si="92"/>
+        <f t="shared" si="96"/>
         <v>0.10104803752746273</v>
       </c>
       <c r="Y42" s="7">
-        <f t="shared" si="92"/>
+        <f t="shared" si="96"/>
         <v>8.5767038180078442E-2</v>
       </c>
       <c r="Z42" s="7">
-        <f t="shared" si="92"/>
+        <f t="shared" si="96"/>
         <v>8.9371990598870577E-2</v>
       </c>
       <c r="AA42" s="7">
-        <f t="shared" si="92"/>
+        <f t="shared" si="96"/>
         <v>0.08</v>
       </c>
       <c r="AB42" s="7">
-        <f t="shared" si="92"/>
+        <f t="shared" si="96"/>
         <v>0.08</v>
       </c>
       <c r="AC42" s="7">
-        <f t="shared" si="92"/>
+        <f t="shared" si="96"/>
         <v>0.08</v>
       </c>
       <c r="AD42" s="7">
-        <f t="shared" si="92"/>
+        <f t="shared" si="96"/>
         <v>0.08</v>
       </c>
       <c r="AE42" s="7">
-        <f t="shared" si="92"/>
+        <f t="shared" si="96"/>
         <v>0.08</v>
       </c>
       <c r="AF42" s="7">
-        <f t="shared" si="92"/>
+        <f t="shared" si="96"/>
         <v>0.08</v>
       </c>
       <c r="AG42" s="7">
-        <f t="shared" si="92"/>
+        <f t="shared" si="96"/>
         <v>0.08</v>
       </c>
       <c r="AH42" s="7">
-        <f t="shared" si="92"/>
+        <f t="shared" si="96"/>
         <v>0.08</v>
       </c>
       <c r="AI42" s="7">
-        <f t="shared" si="92"/>
+        <f t="shared" si="96"/>
         <v>0.08</v>
       </c>
       <c r="AJ42" s="7">
-        <f t="shared" si="92"/>
+        <f t="shared" si="96"/>
         <v>0.08</v>
       </c>
       <c r="AM42" s="1" t="s">
@@ -5702,39 +5702,39 @@
         <v>52</v>
       </c>
       <c r="C43" s="7">
-        <f t="shared" ref="C43:K43" si="93">C25/C16</f>
+        <f t="shared" ref="C43:K43" si="97">C25/C16</f>
         <v>0.22495023224950234</v>
       </c>
       <c r="D43" s="7">
-        <f t="shared" si="93"/>
+        <f t="shared" si="97"/>
         <v>0.18382246638716207</v>
       </c>
       <c r="E43" s="7">
-        <f t="shared" si="93"/>
+        <f t="shared" si="97"/>
         <v>0.171335005574136</v>
       </c>
       <c r="F43" s="7">
-        <f t="shared" si="93"/>
+        <f t="shared" si="97"/>
         <v>0.12162777091594618</v>
       </c>
       <c r="G43" s="7">
-        <f t="shared" si="93"/>
+        <f t="shared" si="97"/>
         <v>0.13790250731831488</v>
       </c>
       <c r="H43" s="7">
-        <f t="shared" si="93"/>
+        <f t="shared" si="97"/>
         <v>0.16347763692896436</v>
       </c>
       <c r="I43" s="7">
-        <f t="shared" si="93"/>
+        <f t="shared" si="97"/>
         <v>0.18045287851446534</v>
       </c>
       <c r="J43" s="7">
-        <f t="shared" si="93"/>
+        <f t="shared" si="97"/>
         <v>0.14154504986758326</v>
       </c>
       <c r="K43" s="7">
-        <f t="shared" si="93"/>
+        <f t="shared" si="97"/>
         <v>0.17661593755264784</v>
       </c>
       <c r="L43" s="7">
@@ -5742,87 +5742,87 @@
         <v>0.20601184975811274</v>
       </c>
       <c r="M43" s="7">
-        <f t="shared" ref="M43:N43" si="94">M25/M16</f>
+        <f t="shared" ref="M43:N43" si="98">M25/M16</f>
         <v>0.17061611374407584</v>
       </c>
       <c r="N43" s="7">
-        <f t="shared" si="94"/>
+        <f t="shared" si="98"/>
         <v>0.14340722239567072</v>
       </c>
       <c r="O43" s="7">
-        <f t="shared" ref="O43:R43" si="95">O25/O16</f>
+        <f t="shared" ref="O43:R43" si="99">O25/O16</f>
         <v>0.17588337822848993</v>
       </c>
       <c r="P43" s="7">
-        <f t="shared" si="95"/>
+        <f t="shared" si="99"/>
         <v>0.19179341248181694</v>
       </c>
       <c r="Q43" s="7">
-        <f t="shared" si="95"/>
+        <f t="shared" si="99"/>
         <v>0.18545992299508895</v>
       </c>
       <c r="R43" s="7">
-        <f t="shared" si="95"/>
+        <f t="shared" si="99"/>
         <v>0.1446621554906895</v>
       </c>
       <c r="V43" s="7">
-        <f t="shared" ref="V43:AJ43" si="96">V25/V16</f>
+        <f t="shared" ref="V43:AJ43" si="100">V25/V16</f>
         <v>0.26846217895343621</v>
       </c>
       <c r="W43" s="7">
-        <f t="shared" si="96"/>
+        <f t="shared" si="100"/>
         <v>0.17231460674157303</v>
       </c>
       <c r="X43" s="7">
-        <f t="shared" si="96"/>
+        <f t="shared" si="100"/>
         <v>0.15606258535716405</v>
       </c>
       <c r="Y43" s="7">
-        <f t="shared" si="96"/>
+        <f t="shared" si="100"/>
         <v>0.17378471988248137</v>
       </c>
       <c r="Z43" s="7">
-        <f t="shared" si="96"/>
+        <f t="shared" si="100"/>
         <v>0.17426523592788018</v>
       </c>
       <c r="AA43" s="7">
-        <f t="shared" si="96"/>
+        <f t="shared" si="100"/>
         <v>0.18688694885786039</v>
       </c>
       <c r="AB43" s="7">
-        <f t="shared" si="96"/>
+        <f t="shared" si="100"/>
         <v>0.18831958124773465</v>
       </c>
       <c r="AC43" s="7">
-        <f t="shared" si="96"/>
+        <f t="shared" si="100"/>
         <v>0.18918504723267354</v>
       </c>
       <c r="AD43" s="7">
-        <f t="shared" si="96"/>
+        <f t="shared" si="100"/>
         <v>0.18960383116562732</v>
       </c>
       <c r="AE43" s="7">
-        <f t="shared" si="96"/>
+        <f t="shared" si="100"/>
         <v>0.18988930495721318</v>
       </c>
       <c r="AF43" s="7">
-        <f t="shared" si="96"/>
+        <f t="shared" si="100"/>
         <v>0.19003424427466581</v>
       </c>
       <c r="AG43" s="7">
-        <f t="shared" si="96"/>
+        <f t="shared" si="100"/>
         <v>0.19018019331968872</v>
       </c>
       <c r="AH43" s="7">
-        <f t="shared" si="96"/>
+        <f t="shared" si="100"/>
         <v>0.19032715552301208</v>
       </c>
       <c r="AI43" s="7">
-        <f t="shared" si="96"/>
+        <f t="shared" si="100"/>
         <v>0.19047513426413587</v>
       </c>
       <c r="AJ43" s="7">
-        <f t="shared" si="96"/>
+        <f t="shared" si="100"/>
         <v>0.19062413287011915</v>
       </c>
       <c r="AM43" s="1" t="s">
@@ -5838,39 +5838,39 @@
         <v>33</v>
       </c>
       <c r="C44" s="7">
-        <f t="shared" ref="C44:K44" si="97">C26/C25</f>
+        <f t="shared" ref="C44:K44" si="101">C26/C25</f>
         <v>0.22603244837758113</v>
       </c>
       <c r="D44" s="7">
-        <f t="shared" si="97"/>
+        <f t="shared" si="101"/>
         <v>0.22768383798662997</v>
       </c>
       <c r="E44" s="7">
-        <f t="shared" si="97"/>
+        <f t="shared" si="101"/>
         <v>0.23586823912159413</v>
       </c>
       <c r="F44" s="7">
-        <f t="shared" si="97"/>
+        <f t="shared" si="101"/>
         <v>0.15980758952431853</v>
       </c>
       <c r="G44" s="7">
-        <f t="shared" si="97"/>
+        <f t="shared" si="101"/>
         <v>0.16197508075680664</v>
       </c>
       <c r="H44" s="7">
-        <f t="shared" si="97"/>
+        <f t="shared" si="101"/>
         <v>0.20482809070958302</v>
       </c>
       <c r="I44" s="7">
-        <f t="shared" si="97"/>
+        <f t="shared" si="101"/>
         <v>0.20935483870967742</v>
       </c>
       <c r="J44" s="7">
-        <f t="shared" si="97"/>
+        <f t="shared" si="101"/>
         <v>0.2304936305732484</v>
       </c>
       <c r="K44" s="7">
-        <f t="shared" si="97"/>
+        <f t="shared" si="101"/>
         <v>0.22511923688394275</v>
       </c>
       <c r="L44" s="7">
@@ -5878,87 +5878,87 @@
         <v>0.20448548812664907</v>
       </c>
       <c r="M44" s="7">
-        <f t="shared" ref="M44:N44" si="98">M26/M25</f>
+        <f t="shared" ref="M44:N44" si="102">M26/M25</f>
         <v>0.21754057428214732</v>
       </c>
       <c r="N44" s="7">
-        <f t="shared" si="98"/>
+        <f t="shared" si="102"/>
         <v>0.21262699564586357</v>
       </c>
       <c r="O44" s="7">
-        <f t="shared" ref="O44:R44" si="99">O26/O25</f>
+        <f t="shared" ref="O44:R44" si="103">O26/O25</f>
         <v>0.22402402402402402</v>
       </c>
       <c r="P44" s="7">
-        <f t="shared" si="99"/>
+        <f t="shared" si="103"/>
         <v>0.21</v>
       </c>
       <c r="Q44" s="7">
-        <f t="shared" si="99"/>
+        <f t="shared" si="103"/>
         <v>0.21</v>
       </c>
       <c r="R44" s="7">
-        <f t="shared" si="99"/>
+        <f t="shared" si="103"/>
         <v>0.21</v>
       </c>
       <c r="V44" s="7">
-        <f t="shared" ref="V44:AJ44" si="100">V26/V25</f>
+        <f t="shared" ref="V44:AJ44" si="104">V26/V25</f>
         <v>0.24358821424311106</v>
       </c>
       <c r="W44" s="7">
-        <f t="shared" si="100"/>
+        <f t="shared" si="104"/>
         <v>0.21606677099634847</v>
       </c>
       <c r="X44" s="7">
-        <f t="shared" si="100"/>
+        <f t="shared" si="104"/>
         <v>0.20346237991058688</v>
       </c>
       <c r="Y44" s="7">
-        <f t="shared" si="100"/>
+        <f t="shared" si="104"/>
         <v>0.21450174486234974</v>
       </c>
       <c r="Z44" s="7">
-        <f t="shared" si="100"/>
+        <f t="shared" si="104"/>
         <v>0.2134124402005477</v>
       </c>
       <c r="AA44" s="7">
-        <f t="shared" si="100"/>
+        <f t="shared" si="104"/>
         <v>0.2</v>
       </c>
       <c r="AB44" s="7">
-        <f t="shared" si="100"/>
+        <f t="shared" si="104"/>
         <v>0.2</v>
       </c>
       <c r="AC44" s="7">
-        <f t="shared" si="100"/>
+        <f t="shared" si="104"/>
         <v>0.2</v>
       </c>
       <c r="AD44" s="7">
-        <f t="shared" si="100"/>
+        <f t="shared" si="104"/>
         <v>0.2</v>
       </c>
       <c r="AE44" s="7">
-        <f t="shared" si="100"/>
+        <f t="shared" si="104"/>
         <v>0.2</v>
       </c>
       <c r="AF44" s="7">
-        <f t="shared" si="100"/>
+        <f t="shared" si="104"/>
         <v>0.2</v>
       </c>
       <c r="AG44" s="7">
-        <f t="shared" si="100"/>
+        <f t="shared" si="104"/>
         <v>0.2</v>
       </c>
       <c r="AH44" s="7">
-        <f t="shared" si="100"/>
+        <f t="shared" si="104"/>
         <v>0.2</v>
       </c>
       <c r="AI44" s="7">
-        <f t="shared" si="100"/>
+        <f t="shared" si="104"/>
         <v>0.2</v>
       </c>
       <c r="AJ44" s="7">
-        <f t="shared" si="100"/>
+        <f t="shared" si="104"/>
         <v>0.2</v>
       </c>
       <c r="AM44" s="1" t="s">
@@ -5974,39 +5974,39 @@
         <v>53</v>
       </c>
       <c r="C45" s="7">
-        <f t="shared" ref="C45:K45" si="101">C27/C16</f>
+        <f t="shared" ref="C45:K45" si="105">C27/C16</f>
         <v>0.17410418049104182</v>
       </c>
       <c r="D45" s="7">
-        <f t="shared" si="101"/>
+        <f t="shared" si="105"/>
         <v>0.14196906173196472</v>
       </c>
       <c r="E45" s="7">
-        <f t="shared" si="101"/>
+        <f t="shared" si="105"/>
         <v>0.13092251950947603</v>
       </c>
       <c r="F45" s="7">
-        <f t="shared" si="101"/>
+        <f t="shared" si="105"/>
         <v>0.1021907300266528</v>
       </c>
       <c r="G45" s="7">
-        <f t="shared" si="101"/>
+        <f t="shared" si="105"/>
         <v>0.11556573755886471</v>
       </c>
       <c r="H45" s="7">
-        <f t="shared" si="101"/>
+        <f t="shared" si="105"/>
         <v>0.12999282468309017</v>
       </c>
       <c r="I45" s="7">
-        <f t="shared" si="101"/>
+        <f t="shared" si="105"/>
         <v>0.14267419523837244</v>
       </c>
       <c r="J45" s="7">
-        <f t="shared" si="101"/>
+        <f t="shared" si="105"/>
         <v>0.10891981743393249</v>
       </c>
       <c r="K45" s="7">
-        <f t="shared" si="101"/>
+        <f t="shared" si="105"/>
         <v>0.13685629246925365</v>
       </c>
       <c r="L45" s="7">
@@ -6014,87 +6014,87 @@
         <v>0.16388541610045115</v>
       </c>
       <c r="M45" s="7">
-        <f t="shared" ref="M45:N45" si="102">M27/M16</f>
+        <f t="shared" ref="M45:N45" si="106">M27/M16</f>
         <v>0.13350018637840141</v>
       </c>
       <c r="N45" s="7">
-        <f t="shared" si="102"/>
+        <f t="shared" si="106"/>
         <v>0.11291497554376105</v>
       </c>
       <c r="O45" s="7">
-        <f t="shared" ref="O45:R45" si="103">O27/O16</f>
+        <f t="shared" ref="O45:R45" si="107">O27/O16</f>
         <v>0.1364812760788042</v>
       </c>
       <c r="P45" s="7">
-        <f t="shared" si="103"/>
+        <f t="shared" si="107"/>
         <v>0.15151679586063538</v>
       </c>
       <c r="Q45" s="7">
-        <f t="shared" si="103"/>
+        <f t="shared" si="107"/>
         <v>0.14651333916612028</v>
       </c>
       <c r="R45" s="7">
-        <f t="shared" si="103"/>
+        <f t="shared" si="107"/>
         <v>0.1142831028376447</v>
       </c>
       <c r="V45" s="7">
-        <f t="shared" ref="V45:AJ45" si="104">V27/V16</f>
+        <f t="shared" ref="V45:AJ45" si="108">V27/V16</f>
         <v>0.2030679561903542</v>
       </c>
       <c r="W45" s="7">
-        <f t="shared" si="104"/>
+        <f t="shared" si="108"/>
         <v>0.13508314606741573</v>
       </c>
       <c r="X45" s="7">
-        <f t="shared" si="104"/>
+        <f t="shared" si="108"/>
         <v>0.12430972032539635</v>
       </c>
       <c r="Y45" s="7">
-        <f t="shared" si="104"/>
+        <f t="shared" si="108"/>
         <v>0.13650759423727443</v>
       </c>
       <c r="Z45" s="7">
-        <f t="shared" si="104"/>
+        <f t="shared" si="108"/>
         <v>0.1370748666863871</v>
       </c>
       <c r="AA45" s="7">
-        <f t="shared" si="104"/>
+        <f t="shared" si="108"/>
         <v>0.14950955908628832</v>
       </c>
       <c r="AB45" s="7">
-        <f t="shared" si="104"/>
+        <f t="shared" si="108"/>
         <v>0.15065566499818772</v>
       </c>
       <c r="AC45" s="7">
-        <f t="shared" si="104"/>
+        <f t="shared" si="108"/>
         <v>0.15134803778613884</v>
       </c>
       <c r="AD45" s="7">
-        <f t="shared" si="104"/>
+        <f t="shared" si="108"/>
         <v>0.15168306493250183</v>
       </c>
       <c r="AE45" s="7">
-        <f t="shared" si="104"/>
+        <f t="shared" si="108"/>
         <v>0.15191144396577055</v>
       </c>
       <c r="AF45" s="7">
-        <f t="shared" si="104"/>
+        <f t="shared" si="108"/>
         <v>0.15202739541973262</v>
       </c>
       <c r="AG45" s="7">
-        <f t="shared" si="104"/>
+        <f t="shared" si="108"/>
         <v>0.15214415465575096</v>
       </c>
       <c r="AH45" s="7">
-        <f t="shared" si="104"/>
+        <f t="shared" si="108"/>
         <v>0.15226172441840968</v>
       </c>
       <c r="AI45" s="7">
-        <f t="shared" si="104"/>
+        <f t="shared" si="108"/>
         <v>0.1523801074113087</v>
       </c>
       <c r="AJ45" s="7">
-        <f t="shared" si="104"/>
+        <f t="shared" si="108"/>
         <v>0.15249930629609529</v>
       </c>
       <c r="AM45" s="1" t="s">

</xml_diff>